<commit_message>
Installation function is working and finished
</commit_message>
<xml_diff>
--- a/Printers drivers.xlsx
+++ b/Printers drivers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\l.oeslick\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\GitHub\iSh0ck\Vela31 - Ineo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6ED061-B503-4C94-B479-2F71099C529F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7467C02F-5264-4395-92D8-884933833C30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{BA73FD97-BD86-4607-825E-05ABED5382E8}"/>
+    <workbookView xWindow="4725" yWindow="7035" windowWidth="19380" windowHeight="9375" xr2:uid="{BA73FD97-BD86-4607-825E-05ABED5382E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -351,7 +351,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -380,7 +380,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -530,33 +530,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color theme="1" tint="0.79998168889431442"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color theme="1" tint="0.79998168889431442"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color theme="1" tint="0.79998168889431442"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -568,8 +546,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -592,6 +568,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -608,10 +652,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="9CA5BC"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="161A21"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -900,13 +944,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75195DAF-320D-408A-B568-5732F052AE7B}">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="31.85546875" customWidth="1"/>
@@ -919,12 +963,12 @@
     <col min="9" max="9" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1">
       <c r="A2" s="4" t="s">
         <v>30</v>
       </c>
@@ -936,33 +980,33 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:9" ht="15.75" thickTop="1">
+      <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>68</v>
       </c>
@@ -984,7 +1028,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="5" t="s">
         <v>31</v>
       </c>
@@ -1002,7 +1046,7 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="5" t="s">
         <v>32</v>
       </c>
@@ -1020,464 +1064,341 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="8"/>
+      <c r="B9" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H9" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickTop="1">
       <c r="A10" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="8"/>
+      <c r="B10" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" s="16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>78</v>
-      </c>
+      <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3" t="s">
-        <v>84</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F14" s="3"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>82</v>
-      </c>
+      <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
-        <v>76</v>
+        <v>102</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="1"/>
+      <c r="H15" s="3"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="15.75" thickTop="1">
       <c r="A16" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="1"/>
+      <c r="B16" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="15.75" thickBot="1">
       <c r="A17" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="1"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>92</v>
+      </c>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
       <c r="A18" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="1"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="F18" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G18" t="s">
+        <v>94</v>
+      </c>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="15.75" thickTop="1">
       <c r="A19" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="1"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="A20" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="1"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="1"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="1"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="1"/>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9">
       <c r="A24" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="12"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="A25" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F25" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G25" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="H25" s="16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-    </row>
-    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="3"/>
-    </row>
-    <row r="33" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:1" ht="15.75" thickBot="1">
       <c r="A33" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B33" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="E33" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G33" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="H33" s="14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="8"/>
-      <c r="C34" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E34" s="8"/>
-      <c r="F34" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G34" s="18" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="8"/>
-      <c r="C35" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="E35" s="10"/>
-      <c r="F35" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="G35" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="34" spans="1:1" ht="15.75" thickTop="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>